<commit_message>
Addition of Spike Isolation
</commit_message>
<xml_diff>
--- a/documentation/Results.xlsx
+++ b/documentation/Results.xlsx
@@ -1,62 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srdjan/MATLAB/projects/project_b/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srdja\MATLAB\Projects\project_b\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2DCC3E-9D07-1446-A7C7-72E5B416C1F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F384F2A9-0395-432D-B171-848F9F7A82C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{33BD343B-4DA1-8C49-B7ED-CCD67F2B21EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{33BD343B-4DA1-8C49-B7ED-CCD67F2B21EB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Breakdown" sheetId="5" r:id="rId1"/>
+    <sheet name="Overlapped" sheetId="6" r:id="rId1"/>
+    <sheet name="Breakdown" sheetId="5" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Breakdown!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Breakdown!$F$22:$F$23</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Breakdown!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Breakdown!$F$22:$F$23</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Breakdown!$F$24:$F$40</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Breakdown!$I$22:$I$23</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Breakdown!$I$24:$I$40</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Breakdown!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Breakdown!$F$22:$F$23</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Breakdown!$F$24:$F$40</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Breakdown!$I$22:$I$23</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Breakdown!$I$24:$I$40</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Breakdown!$F$24:$F$39</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Breakdown!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Breakdown!$F$22:$F$23</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Breakdown!$F$24:$F$39</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Breakdown!$I$22:$I$23</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Breakdown!$I$24:$I$39</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Breakdown!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Breakdown!$F$22:$F$23</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Breakdown!$F$24:$F$39</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Breakdown!$I$22:$I$23</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Breakdown!$I$24:$I$39</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Breakdown!$I$22:$I$23</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Breakdown!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Breakdown!$F$22:$F$23</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Breakdown!$F$24:$F$39</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Breakdown!$I$22:$I$23</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Breakdown!$I$24:$I$39</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Breakdown!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Breakdown!$F$22:$F$23</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Breakdown!$F$24:$F$39</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Breakdown!$I$22:$I$23</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Breakdown!$I$24:$I$39</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Breakdown!$I$24:$I$39</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Breakdown!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Breakdown!$F$22:$F$23</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Breakdown!$F$24:$F$40</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Breakdown!$I$22:$I$23</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Breakdown!$I$24:$I$40</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -65,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -75,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="31">
   <si>
     <t>C_Easy1_noise005</t>
   </si>
@@ -166,13 +123,16 @@
   <si>
     <t>Pr(Overlapped)</t>
   </si>
+  <si>
+    <t>Precision Improvements</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -354,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -381,15 +341,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -400,48 +351,60 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,7 +427,535 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>Average Improvements </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26184692997995801"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overlapped!$F$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Without STM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="84000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Overlapped!$I$23:$K$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Precision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Recall</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overlapped!$F$40:$H$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.64971134918501428</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41241524466109286</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32927789920259698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67DA-40AA-A5FB-63C502DA257A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overlapped!$I$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>With STM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="84000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Overlapped!$I$23:$K$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Precision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Recall</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overlapped!$I$40:$K$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.75217767178628892</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48099441289470696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40846729791449954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-67DA-40AA-A5FB-63C502DA257A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="41"/>
+        <c:axId val="327252559"/>
+        <c:axId val="348881871"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="327252559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348881871"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="348881871"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="327252559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="68000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+      </a:gsLst>
+      <a:lin ang="5400000" scaled="1"/>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1025,6 +1516,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="204">
   <cs:axisTitle>
@@ -1592,7 +2123,617 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="204">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200">
+      <a:effectLst/>
+    </cs:defRPr>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="68000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="84000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr kern="1200">
+      <a:effectLst/>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09A05D98-0BF1-4D1E-ACFB-19ACD7338CA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1929,45 +3070,1245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20518AC8-BF6B-4806-BF77-65F98C6B00A3}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="C2:O40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F2" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="37"/>
+      <c r="K2" s="38"/>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4">
+        <v>259</v>
+      </c>
+      <c r="F4" s="2">
+        <v>125</v>
+      </c>
+      <c r="G4" s="4">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1">
+        <v>134</v>
+      </c>
+      <c r="I4" s="2">
+        <v>134</v>
+      </c>
+      <c r="J4" s="4">
+        <v>16</v>
+      </c>
+      <c r="K4" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4">
+        <v>241</v>
+      </c>
+      <c r="F5" s="2">
+        <v>112</v>
+      </c>
+      <c r="G5" s="4">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1">
+        <v>129</v>
+      </c>
+      <c r="I5" s="2">
+        <v>116</v>
+      </c>
+      <c r="J5" s="4">
+        <v>18</v>
+      </c>
+      <c r="K5" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4">
+        <v>262</v>
+      </c>
+      <c r="F6" s="2">
+        <v>72</v>
+      </c>
+      <c r="G6" s="4">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
+        <v>190</v>
+      </c>
+      <c r="I6" s="2">
+        <v>79</v>
+      </c>
+      <c r="J6" s="4">
+        <v>13</v>
+      </c>
+      <c r="K6" s="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4">
+        <v>264</v>
+      </c>
+      <c r="F7" s="2">
+        <v>22</v>
+      </c>
+      <c r="G7" s="4">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>242</v>
+      </c>
+      <c r="I7" s="2">
+        <v>29</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4">
+        <v>256</v>
+      </c>
+      <c r="F8" s="2">
+        <v>148</v>
+      </c>
+      <c r="G8" s="4">
+        <v>79</v>
+      </c>
+      <c r="H8" s="1">
+        <v>108</v>
+      </c>
+      <c r="I8" s="2">
+        <v>176</v>
+      </c>
+      <c r="J8" s="4">
+        <v>51</v>
+      </c>
+      <c r="K8" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4">
+        <v>285</v>
+      </c>
+      <c r="F9" s="2">
+        <v>150</v>
+      </c>
+      <c r="G9" s="4">
+        <v>95</v>
+      </c>
+      <c r="H9" s="1">
+        <v>135</v>
+      </c>
+      <c r="I9" s="2">
+        <v>183</v>
+      </c>
+      <c r="J9" s="4">
+        <v>62</v>
+      </c>
+      <c r="K9" s="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4">
+        <v>242</v>
+      </c>
+      <c r="F10" s="2">
+        <v>109</v>
+      </c>
+      <c r="G10" s="4">
+        <v>135</v>
+      </c>
+      <c r="H10" s="1">
+        <v>133</v>
+      </c>
+      <c r="I10" s="2">
+        <v>130</v>
+      </c>
+      <c r="J10" s="4">
+        <v>114</v>
+      </c>
+      <c r="K10" s="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4">
+        <v>224</v>
+      </c>
+      <c r="F11" s="2">
+        <v>67</v>
+      </c>
+      <c r="G11" s="4">
+        <v>112</v>
+      </c>
+      <c r="H11" s="1">
+        <v>157</v>
+      </c>
+      <c r="I11" s="2">
+        <v>87</v>
+      </c>
+      <c r="J11" s="4">
+        <v>92</v>
+      </c>
+      <c r="K11" s="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4">
+        <v>18</v>
+      </c>
+      <c r="E12" s="4">
+        <v>249</v>
+      </c>
+      <c r="F12" s="2">
+        <v>172</v>
+      </c>
+      <c r="G12" s="4">
+        <v>42</v>
+      </c>
+      <c r="H12" s="1">
+        <v>77</v>
+      </c>
+      <c r="I12" s="2">
+        <v>206</v>
+      </c>
+      <c r="J12" s="4">
+        <v>8</v>
+      </c>
+      <c r="K12" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4">
+        <v>9</v>
+      </c>
+      <c r="E13" s="4">
+        <v>243</v>
+      </c>
+      <c r="F13" s="2">
+        <v>147</v>
+      </c>
+      <c r="G13" s="4">
+        <v>38</v>
+      </c>
+      <c r="H13" s="1">
+        <v>96</v>
+      </c>
+      <c r="I13" s="2">
+        <v>167</v>
+      </c>
+      <c r="J13" s="4">
+        <v>18</v>
+      </c>
+      <c r="K13" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4">
+        <v>262</v>
+      </c>
+      <c r="F14" s="2">
+        <v>92</v>
+      </c>
+      <c r="G14" s="4">
+        <v>39</v>
+      </c>
+      <c r="H14" s="1">
+        <v>170</v>
+      </c>
+      <c r="I14" s="2">
+        <v>110</v>
+      </c>
+      <c r="J14" s="4">
+        <v>21</v>
+      </c>
+      <c r="K14" s="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="4">
+        <v>6</v>
+      </c>
+      <c r="E15" s="4">
+        <v>243</v>
+      </c>
+      <c r="F15" s="2">
+        <v>19</v>
+      </c>
+      <c r="G15" s="4">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1">
+        <v>224</v>
+      </c>
+      <c r="I15" s="2">
+        <v>20</v>
+      </c>
+      <c r="J15" s="4">
+        <v>12</v>
+      </c>
+      <c r="K15" s="1">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="4">
+        <v>18</v>
+      </c>
+      <c r="E16" s="4">
+        <v>265</v>
+      </c>
+      <c r="F16" s="2">
+        <v>140</v>
+      </c>
+      <c r="G16" s="4">
+        <v>121</v>
+      </c>
+      <c r="H16" s="1">
+        <v>125</v>
+      </c>
+      <c r="I16" s="2">
+        <v>179</v>
+      </c>
+      <c r="J16" s="4">
+        <v>82</v>
+      </c>
+      <c r="K16" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4">
+        <v>204</v>
+      </c>
+      <c r="F17" s="2">
+        <v>116</v>
+      </c>
+      <c r="G17" s="4">
+        <v>104</v>
+      </c>
+      <c r="H17" s="1">
+        <v>88</v>
+      </c>
+      <c r="I17" s="2">
+        <v>137</v>
+      </c>
+      <c r="J17" s="4">
+        <v>83</v>
+      </c>
+      <c r="K17" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4">
+        <v>264</v>
+      </c>
+      <c r="F18" s="2">
+        <v>113</v>
+      </c>
+      <c r="G18" s="4">
+        <v>62</v>
+      </c>
+      <c r="H18" s="1">
+        <v>151</v>
+      </c>
+      <c r="I18" s="2">
+        <v>120</v>
+      </c>
+      <c r="J18" s="4">
+        <v>55</v>
+      </c>
+      <c r="K18" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4">
+        <v>6</v>
+      </c>
+      <c r="E19" s="4">
+        <v>259</v>
+      </c>
+      <c r="F19" s="2">
+        <v>49</v>
+      </c>
+      <c r="G19" s="4">
+        <v>45</v>
+      </c>
+      <c r="H19" s="1">
+        <v>210</v>
+      </c>
+      <c r="I19" s="2">
+        <v>55</v>
+      </c>
+      <c r="J19" s="4">
+        <v>39</v>
+      </c>
+      <c r="K19" s="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="11">
+        <f>AVERAGE(F4:F19)</f>
+        <v>103.3125</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" ref="G20:K20" si="0">AVERAGE(G4:G19)</f>
+        <v>60</v>
+      </c>
+      <c r="H20" s="13">
+        <f t="shared" si="0"/>
+        <v>148.0625</v>
+      </c>
+      <c r="I20" s="11">
+        <f t="shared" si="0"/>
+        <v>120.5</v>
+      </c>
+      <c r="J20" s="12">
+        <f t="shared" si="0"/>
+        <v>42.8125</v>
+      </c>
+      <c r="K20" s="13">
+        <f t="shared" si="0"/>
+        <v>130.875</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="F22" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="37"/>
+      <c r="K22" s="38"/>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>16</v>
+      </c>
+      <c r="E24" s="4">
+        <v>3514</v>
+      </c>
+      <c r="F24" s="20">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="G24" s="21">
+        <v>0.48262548262548299</v>
+      </c>
+      <c r="H24" s="22">
+        <v>0.440140845070423</v>
+      </c>
+      <c r="I24" s="20">
+        <v>0.89333333333333298</v>
+      </c>
+      <c r="J24" s="21">
+        <v>0.51737451737451701</v>
+      </c>
+      <c r="K24" s="22">
+        <v>0.48727272727272702</v>
+      </c>
+      <c r="L24" s="35">
+        <f>I24-F24</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4">
+        <v>9</v>
+      </c>
+      <c r="E25" s="4">
+        <v>3522</v>
+      </c>
+      <c r="F25" s="23">
+        <v>0.83582089552238803</v>
+      </c>
+      <c r="G25" s="24">
+        <v>0.46473029045643199</v>
+      </c>
+      <c r="H25" s="25">
+        <v>0.42585551330798499</v>
+      </c>
+      <c r="I25" s="23">
+        <v>0.86567164179104505</v>
+      </c>
+      <c r="J25" s="24">
+        <v>0.48132780082987597</v>
+      </c>
+      <c r="K25" s="25">
+        <v>0.44787644787644798</v>
+      </c>
+      <c r="L25" s="35">
+        <f t="shared" ref="L25:L39" si="1">I25-F25</f>
+        <v>2.9850746268657025E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4">
+        <v>6</v>
+      </c>
+      <c r="E26" s="4">
+        <v>3477</v>
+      </c>
+      <c r="F26" s="23">
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="G26" s="24">
+        <v>0.27480916030534402</v>
+      </c>
+      <c r="H26" s="25">
+        <v>0.25531914893617003</v>
+      </c>
+      <c r="I26" s="23">
+        <v>0.85869565217391297</v>
+      </c>
+      <c r="J26" s="24">
+        <v>0.30152671755725202</v>
+      </c>
+      <c r="K26" s="25">
+        <v>0.28727272727272701</v>
+      </c>
+      <c r="L26" s="35">
+        <f t="shared" si="1"/>
+        <v>7.6086956521739024E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4">
+        <v>6</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3474</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="G27" s="24">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H27" s="25">
+        <v>8.0882352941176502E-2</v>
+      </c>
+      <c r="I27" s="23">
+        <v>0.96666666666666701</v>
+      </c>
+      <c r="J27" s="24">
+        <v>0.109848484848485</v>
+      </c>
+      <c r="K27" s="25">
+        <v>0.109433962264151</v>
+      </c>
+      <c r="L27" s="35">
+        <f t="shared" si="1"/>
+        <v>0.23333333333333406</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="4">
+        <v>19</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3410</v>
+      </c>
+      <c r="F28" s="23">
+        <v>0.65198237885462595</v>
+      </c>
+      <c r="G28" s="24">
+        <v>0.578125</v>
+      </c>
+      <c r="H28" s="25">
+        <v>0.44179104477611902</v>
+      </c>
+      <c r="I28" s="23">
+        <v>0.77533039647577096</v>
+      </c>
+      <c r="J28" s="24">
+        <v>0.6875</v>
+      </c>
+      <c r="K28" s="25">
+        <v>0.57328990228012999</v>
+      </c>
+      <c r="L28" s="35">
+        <f t="shared" si="1"/>
+        <v>0.123348017621145</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="4">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4">
+        <v>3520</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.61224489795918402</v>
+      </c>
+      <c r="G29" s="24">
+        <v>0.52631578947368396</v>
+      </c>
+      <c r="H29" s="25">
+        <v>0.394736842105263</v>
+      </c>
+      <c r="I29" s="23">
+        <v>0.74693877551020404</v>
+      </c>
+      <c r="J29" s="24">
+        <v>0.64210526315789496</v>
+      </c>
+      <c r="K29" s="25">
+        <v>0.527377521613833</v>
+      </c>
+      <c r="L29" s="35">
+        <f t="shared" si="1"/>
+        <v>0.13469387755102002</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="4">
+        <v>7</v>
+      </c>
+      <c r="E30" s="4">
+        <v>3411</v>
+      </c>
+      <c r="F30" s="23">
+        <v>0.44672131147541</v>
+      </c>
+      <c r="G30" s="24">
+        <v>0.45041322314049598</v>
+      </c>
+      <c r="H30" s="25">
+        <v>0.289124668435013</v>
+      </c>
+      <c r="I30" s="23">
+        <v>0.53278688524590201</v>
+      </c>
+      <c r="J30" s="24">
+        <v>0.53719008264462798</v>
+      </c>
+      <c r="K30" s="25">
+        <v>0.36516853932584298</v>
+      </c>
+      <c r="L30" s="35">
+        <f t="shared" si="1"/>
+        <v>8.606557377049201E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="4">
+        <v>6</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3526</v>
+      </c>
+      <c r="F31" s="23">
+        <v>0.37430167597765401</v>
+      </c>
+      <c r="G31" s="24">
+        <v>0.29910714285714302</v>
+      </c>
+      <c r="H31" s="25">
+        <v>0.199404761904762</v>
+      </c>
+      <c r="I31" s="23">
+        <v>0.486033519553073</v>
+      </c>
+      <c r="J31" s="24">
+        <v>0.38839285714285698</v>
+      </c>
+      <c r="K31" s="25">
+        <v>0.275316455696203</v>
+      </c>
+      <c r="L31" s="35">
+        <f t="shared" si="1"/>
+        <v>0.11173184357541899</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="4">
+        <v>18</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3383</v>
+      </c>
+      <c r="F32" s="23">
+        <v>0.80373831775700899</v>
+      </c>
+      <c r="G32" s="24">
+        <v>0.69076305220883505</v>
+      </c>
+      <c r="H32" s="25">
+        <v>0.59106529209622005</v>
+      </c>
+      <c r="I32" s="23">
+        <v>0.96261682242990698</v>
+      </c>
+      <c r="J32" s="24">
+        <v>0.82730923694779102</v>
+      </c>
+      <c r="K32" s="25">
+        <v>0.80155642023346296</v>
+      </c>
+      <c r="L32" s="35">
+        <f t="shared" si="1"/>
+        <v>0.15887850467289799</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="4">
+        <v>9</v>
+      </c>
+      <c r="E33" s="4">
+        <v>3448</v>
+      </c>
+      <c r="F33" s="23">
+        <v>0.79459459459459503</v>
+      </c>
+      <c r="G33" s="24">
+        <v>0.60493827160493796</v>
+      </c>
+      <c r="H33" s="25">
+        <v>0.52313167259786497</v>
+      </c>
+      <c r="I33" s="23">
+        <v>0.90270270270270303</v>
+      </c>
+      <c r="J33" s="24">
+        <v>0.687242798353909</v>
+      </c>
+      <c r="K33" s="25">
+        <v>0.639846743295019</v>
+      </c>
+      <c r="L33" s="35">
+        <f t="shared" si="1"/>
+        <v>0.108108108108108</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="4">
+        <v>7</v>
+      </c>
+      <c r="E34" s="4">
+        <v>3472</v>
+      </c>
+      <c r="F34" s="23">
+        <v>0.70229007633587803</v>
+      </c>
+      <c r="G34" s="24">
+        <v>0.35114503816793902</v>
+      </c>
+      <c r="H34" s="25">
+        <v>0.30564784053156102</v>
+      </c>
+      <c r="I34" s="23">
+        <v>0.83969465648855002</v>
+      </c>
+      <c r="J34" s="24">
+        <v>0.41984732824427501</v>
+      </c>
+      <c r="K34" s="25">
+        <v>0.38869257950530001</v>
+      </c>
+      <c r="L34" s="35">
+        <f t="shared" si="1"/>
+        <v>0.13740458015267198</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="4">
+        <v>6</v>
+      </c>
+      <c r="E35" s="4">
+        <v>3414</v>
+      </c>
+      <c r="F35" s="23">
+        <v>0.59375</v>
+      </c>
+      <c r="G35" s="24">
+        <v>7.8189300411522597E-2</v>
+      </c>
+      <c r="H35" s="25">
+        <v>7.421875E-2</v>
+      </c>
+      <c r="I35" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="J35" s="24">
+        <v>8.2304526748971193E-2</v>
+      </c>
+      <c r="K35" s="25">
+        <v>7.8431372549019607E-2</v>
+      </c>
+      <c r="L35" s="35">
+        <f t="shared" si="1"/>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="4">
+        <v>18</v>
+      </c>
+      <c r="E36" s="4">
+        <v>3364</v>
+      </c>
+      <c r="F36" s="23">
+        <v>0.53639846743295005</v>
+      </c>
+      <c r="G36" s="24">
+        <v>0.52830188679245305</v>
+      </c>
+      <c r="H36" s="25">
+        <v>0.362694300518135</v>
+      </c>
+      <c r="I36" s="23">
+        <v>0.68582375478927204</v>
+      </c>
+      <c r="J36" s="24">
+        <v>0.67547169811320795</v>
+      </c>
+      <c r="K36" s="25">
+        <v>0.51585014409221897</v>
+      </c>
+      <c r="L36" s="35">
+        <f t="shared" si="1"/>
+        <v>0.14942528735632199</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="4">
+        <v>10</v>
+      </c>
+      <c r="E37" s="4">
+        <v>3462</v>
+      </c>
+      <c r="F37" s="23">
+        <v>0.527272727272727</v>
+      </c>
+      <c r="G37" s="24">
+        <v>0.56862745098039202</v>
+      </c>
+      <c r="H37" s="25">
+        <v>0.37662337662337703</v>
+      </c>
+      <c r="I37" s="23">
+        <v>0.62272727272727302</v>
+      </c>
+      <c r="J37" s="24">
+        <v>0.67156862745098</v>
+      </c>
+      <c r="K37" s="25">
+        <v>0.47735191637630697</v>
+      </c>
+      <c r="L37" s="35">
+        <f t="shared" si="1"/>
+        <v>9.5454545454546014E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="4">
+        <v>7</v>
+      </c>
+      <c r="E38" s="4">
+        <v>3440</v>
+      </c>
+      <c r="F38" s="23">
+        <v>0.64571428571428602</v>
+      </c>
+      <c r="G38" s="24">
+        <v>0.42803030303030298</v>
+      </c>
+      <c r="H38" s="25">
+        <v>0.34662576687116597</v>
+      </c>
+      <c r="I38" s="23">
+        <v>0.68571428571428605</v>
+      </c>
+      <c r="J38" s="24">
+        <v>0.45454545454545497</v>
+      </c>
+      <c r="K38" s="25">
+        <v>0.37617554858934199</v>
+      </c>
+      <c r="L38" s="35">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="4">
+        <v>6</v>
+      </c>
+      <c r="E39" s="4">
+        <v>3493</v>
+      </c>
+      <c r="F39" s="26">
+        <v>0.52127659574468099</v>
+      </c>
+      <c r="G39" s="27">
+        <v>0.18918918918918901</v>
+      </c>
+      <c r="H39" s="28">
+        <v>0.16118421052631601</v>
+      </c>
+      <c r="I39" s="26">
+        <v>0.58510638297872297</v>
+      </c>
+      <c r="J39" s="27">
+        <v>0.21235521235521199</v>
+      </c>
+      <c r="K39" s="28">
+        <v>0.18456375838926201</v>
+      </c>
+      <c r="L39" s="35">
+        <f t="shared" si="1"/>
+        <v>6.3829787234041979E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C40" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="29">
+        <f>AVERAGE(F24:F39)</f>
+        <v>0.64971134918501428</v>
+      </c>
+      <c r="G40" s="30">
+        <f>AVERAGE(G24:G39)</f>
+        <v>0.41241524466109286</v>
+      </c>
+      <c r="H40" s="30">
+        <f t="shared" ref="H40:K40" si="2">AVERAGE(H24:H39)</f>
+        <v>0.32927789920259698</v>
+      </c>
+      <c r="I40" s="30">
+        <f t="shared" si="2"/>
+        <v>0.75217767178628892</v>
+      </c>
+      <c r="J40" s="30">
+        <f t="shared" si="2"/>
+        <v>0.48099441289470696</v>
+      </c>
+      <c r="K40" s="31">
+        <f t="shared" si="2"/>
+        <v>0.40846729791449954</v>
+      </c>
+      <c r="L40" s="39">
+        <f>MEDIAN(L24:L39)</f>
+        <v>0.10178132678132701</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="30" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16AB61D4-C63B-456F-A0DA-741F75E2D2A6}">
   <dimension ref="C2:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.83203125" customWidth="1"/>
+    <col min="25" max="25" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F2" s="14" t="s">
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="14" t="s">
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
-    </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="J2" s="37"/>
+      <c r="K2" s="38"/>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
@@ -1996,7 +4337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2025,7 +4366,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
@@ -2054,7 +4395,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2083,7 +4424,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
@@ -2112,7 +4453,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -2141,7 +4482,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
@@ -2170,7 +4511,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
@@ -2199,7 +4540,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
@@ -2228,7 +4569,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
@@ -2257,7 +4598,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
@@ -2286,7 +4627,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
@@ -2315,7 +4656,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
@@ -2344,7 +4685,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>12</v>
       </c>
@@ -2373,7 +4714,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>13</v>
       </c>
@@ -2402,7 +4743,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
@@ -2431,7 +4772,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
@@ -2460,7 +4801,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="s">
         <v>25</v>
       </c>
@@ -2491,35 +4832,35 @@
         <v>635.375</v>
       </c>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
-    </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="F22" s="14" t="s">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F22" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="14" t="s">
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="16"/>
-    </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="J22" s="37"/>
+      <c r="K22" s="38"/>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="8" t="s">
         <v>16</v>
       </c>
@@ -2529,32 +4870,32 @@
       <c r="E23" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="18" t="s">
+      <c r="J23" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="17" t="s">
+      <c r="L23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="M23" s="35" t="s">
+      <c r="M23" s="32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>0</v>
       </c>
@@ -2564,39 +4905,39 @@
       <c r="E24" s="4">
         <v>3514</v>
       </c>
-      <c r="F24" s="23">
-        <f>F4/(F4+G4)</f>
+      <c r="F24" s="20">
+        <f t="shared" ref="F24:F39" si="1">F4/(F4+G4)</f>
         <v>0.99049265341400172</v>
       </c>
-      <c r="G24" s="24">
-        <f>F4/(F4+H4)</f>
+      <c r="G24" s="21">
+        <f t="shared" ref="G24:G39" si="2">F4/(F4+H4)</f>
         <v>0.97837222538417756</v>
       </c>
-      <c r="H24" s="25">
-        <f>F4/(F4+G4+H4)</f>
+      <c r="H24" s="22">
+        <f t="shared" ref="H24:H39" si="3">F4/(F4+G4+H4)</f>
         <v>0.96926980546941077</v>
       </c>
-      <c r="I24" s="23">
-        <f>I4/(I4+J4)</f>
+      <c r="I24" s="20">
+        <f t="shared" ref="I24:I39" si="4">I4/(I4+J4)</f>
         <v>0.99308556611927401</v>
       </c>
-      <c r="J24" s="24">
-        <f>I4/(I4+K4)</f>
+      <c r="J24" s="21">
+        <f t="shared" ref="J24:J39" si="5">I4/(I4+K4)</f>
         <v>0.98093340922026184</v>
       </c>
-      <c r="K24" s="25">
-        <f>I4/(I4+J4+K4)</f>
+      <c r="K24" s="22">
+        <f t="shared" ref="K24:K39" si="6">I4/(I4+J4+K4)</f>
         <v>0.97427925381571512</v>
       </c>
-      <c r="L24" s="37">
+      <c r="L24" s="34">
         <f>K24-H24</f>
         <v>5.009448346304346E-3</v>
       </c>
-      <c r="M24" s="38">
+      <c r="M24" s="35">
         <v>2.1895707288965699E-2</v>
       </c>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
@@ -2606,39 +4947,39 @@
       <c r="E25" s="4">
         <v>3522</v>
       </c>
-      <c r="F25" s="26">
-        <f>F5/(F5+G5)</f>
+      <c r="F25" s="23">
+        <f t="shared" si="1"/>
         <v>0.99506244554167878</v>
       </c>
-      <c r="G25" s="27">
-        <f>F5/(F5+H5)</f>
+      <c r="G25" s="24">
+        <f t="shared" si="2"/>
         <v>0.97274275979557068</v>
       </c>
-      <c r="H25" s="28">
-        <f>F5/(F5+G5+H5)</f>
+      <c r="H25" s="25">
+        <f t="shared" si="3"/>
         <v>0.96807007629273811</v>
       </c>
-      <c r="I25" s="26">
-        <f>I5/(I5+J5)</f>
+      <c r="I25" s="23">
+        <f t="shared" si="4"/>
         <v>0.99622422306128378</v>
       </c>
-      <c r="J25" s="27">
-        <f>I5/(I5+K5)</f>
+      <c r="J25" s="24">
+        <f t="shared" si="5"/>
         <v>0.9738784781374219</v>
       </c>
-      <c r="K25" s="28">
-        <f>I5/(I5+J5+K5)</f>
+      <c r="K25" s="25">
+        <f t="shared" si="6"/>
         <v>0.97029702970297027</v>
       </c>
-      <c r="L25" s="37">
-        <f t="shared" ref="L25:L39" si="1">K25-H25</f>
+      <c r="L25" s="34">
+        <f t="shared" ref="L25:L39" si="7">K25-H25</f>
         <v>2.2269534102321575E-3</v>
       </c>
-      <c r="M25" s="38">
+      <c r="M25" s="35">
         <v>1.98789974070873E-2</v>
       </c>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>2</v>
       </c>
@@ -2648,39 +4989,39 @@
       <c r="E26" s="4">
         <v>3477</v>
       </c>
-      <c r="F26" s="26">
-        <f>F6/(F6+G6)</f>
+      <c r="F26" s="23">
+        <f t="shared" si="1"/>
         <v>0.99148936170212765</v>
       </c>
-      <c r="G26" s="27">
-        <f>F6/(F6+H6)</f>
+      <c r="G26" s="24">
+        <f t="shared" si="2"/>
         <v>0.80414150129421913</v>
       </c>
-      <c r="H26" s="28">
-        <f>F6/(F6+G6+H6)</f>
+      <c r="H26" s="25">
+        <f t="shared" si="3"/>
         <v>0.79862896315338472</v>
       </c>
-      <c r="I26" s="26">
-        <f>I6/(I6+J6)</f>
+      <c r="I26" s="23">
+        <f t="shared" si="4"/>
         <v>0.99042553191489358</v>
       </c>
-      <c r="J26" s="27">
-        <f>I6/(I6+K6)</f>
+      <c r="J26" s="24">
+        <f t="shared" si="5"/>
         <v>0.80327868852459017</v>
       </c>
-      <c r="K26" s="28">
-        <f>I6/(I6+J6+K6)</f>
+      <c r="K26" s="25">
+        <f t="shared" si="6"/>
         <v>0.7970890410958904</v>
       </c>
-      <c r="L26" s="37">
-        <f t="shared" si="1"/>
+      <c r="L26" s="34">
+        <f t="shared" si="7"/>
         <v>-1.539922057494314E-3</v>
       </c>
-      <c r="M26" s="38">
+      <c r="M26" s="35">
         <v>1.7862287525208902E-2</v>
       </c>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>3</v>
       </c>
@@ -2690,39 +5031,39 @@
       <c r="E27" s="4">
         <v>3474</v>
       </c>
-      <c r="F27" s="26">
-        <f>F7/(F7+G7)</f>
+      <c r="F27" s="23">
+        <f t="shared" si="1"/>
         <v>0.9713690786048933</v>
       </c>
-      <c r="G27" s="27">
-        <f>F7/(F7+H7)</f>
+      <c r="G27" s="24">
+        <f t="shared" si="2"/>
         <v>0.53713298791018993</v>
       </c>
-      <c r="H27" s="28">
-        <f>F7/(F7+G7+H7)</f>
+      <c r="H27" s="25">
+        <f t="shared" si="3"/>
         <v>0.52876168886370079</v>
       </c>
-      <c r="I27" s="26">
-        <f>I7/(I7+J7)</f>
+      <c r="I27" s="23">
+        <f t="shared" si="4"/>
         <v>0.98438313378448727</v>
       </c>
-      <c r="J27" s="27">
-        <f>I7/(I7+K7)</f>
+      <c r="J27" s="24">
+        <f t="shared" si="5"/>
         <v>0.54432930339666086</v>
       </c>
-      <c r="K27" s="28">
-        <f>I7/(I7+J7+K7)</f>
+      <c r="K27" s="25">
+        <f t="shared" si="6"/>
         <v>0.53966894977168944</v>
       </c>
-      <c r="L27" s="37">
-        <f t="shared" si="1"/>
+      <c r="L27" s="34">
+        <f t="shared" si="7"/>
         <v>1.0907260907988658E-2</v>
       </c>
-      <c r="M27" s="38">
+      <c r="M27" s="35">
         <v>1.41169691731489E-2</v>
       </c>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
         <v>4</v>
       </c>
@@ -2732,39 +5073,39 @@
       <c r="E28" s="4">
         <v>3410</v>
       </c>
-      <c r="F28" s="26">
-        <f>F8/(F8+G8)</f>
+      <c r="F28" s="23">
+        <f t="shared" si="1"/>
         <v>0.98119858989424202</v>
       </c>
-      <c r="G28" s="27">
-        <f>F8/(F8+H8)</f>
+      <c r="G28" s="24">
+        <f t="shared" si="2"/>
         <v>0.97947214076246336</v>
       </c>
-      <c r="H28" s="28">
-        <f>F8/(F8+G8+H8)</f>
+      <c r="H28" s="25">
+        <f t="shared" si="3"/>
         <v>0.96142774899251582</v>
       </c>
-      <c r="I28" s="26">
-        <f>I8/(I8+J8)</f>
+      <c r="I28" s="23">
+        <f t="shared" si="4"/>
         <v>0.98971797884841362</v>
       </c>
-      <c r="J28" s="27">
-        <f>I8/(I8+K8)</f>
+      <c r="J28" s="24">
+        <f t="shared" si="5"/>
         <v>0.98797653958944287</v>
       </c>
-      <c r="K28" s="28">
-        <f>I8/(I8+J8+K8)</f>
+      <c r="K28" s="25">
+        <f t="shared" si="6"/>
         <v>0.9779390420899855</v>
       </c>
-      <c r="L28" s="37">
-        <f t="shared" si="1"/>
+      <c r="L28" s="34">
+        <f t="shared" si="7"/>
         <v>1.6511293097469681E-2</v>
       </c>
-      <c r="M28" s="38">
+      <c r="M28" s="35">
         <v>3.3707865168539297E-2</v>
       </c>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>5</v>
       </c>
@@ -2774,39 +5115,39 @@
       <c r="E29" s="4">
         <v>3520</v>
       </c>
-      <c r="F29" s="26">
-        <f>F9/(F9+G9)</f>
+      <c r="F29" s="23">
+        <f t="shared" si="1"/>
         <v>0.95568181818181819</v>
       </c>
-      <c r="G29" s="27">
-        <f>F9/(F9+H9)</f>
+      <c r="G29" s="24">
+        <f t="shared" si="2"/>
         <v>0.95568181818181819</v>
       </c>
-      <c r="H29" s="28">
-        <f>F9/(F9+G9+H9)</f>
+      <c r="H29" s="25">
+        <f t="shared" si="3"/>
         <v>0.91512513601741019</v>
       </c>
-      <c r="I29" s="26">
-        <f>I9/(I9+J9)</f>
+      <c r="I29" s="23">
+        <f t="shared" si="4"/>
         <v>0.96107954545454544</v>
       </c>
-      <c r="J29" s="27">
-        <f>I9/(I9+K9)</f>
+      <c r="J29" s="24">
+        <f t="shared" si="5"/>
         <v>0.96107954545454544</v>
       </c>
-      <c r="K29" s="28">
-        <f>I9/(I9+J9+K9)</f>
+      <c r="K29" s="25">
+        <f t="shared" si="6"/>
         <v>0.92507519824993167</v>
       </c>
-      <c r="L29" s="37">
-        <f t="shared" si="1"/>
+      <c r="L29" s="34">
+        <f t="shared" si="7"/>
         <v>9.9500622325214838E-3</v>
       </c>
-      <c r="M29" s="38">
+      <c r="M29" s="35">
         <v>3.5227272727272697E-2</v>
       </c>
     </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
         <v>6</v>
       </c>
@@ -2816,39 +5157,39 @@
       <c r="E30" s="4">
         <v>3411</v>
       </c>
-      <c r="F30" s="26">
-        <f>F10/(F10+G10)</f>
+      <c r="F30" s="23">
+        <f t="shared" si="1"/>
         <v>0.8460410557184751</v>
       </c>
-      <c r="G30" s="27">
-        <f>F10/(F10+H10)</f>
+      <c r="G30" s="24">
+        <f t="shared" si="2"/>
         <v>0.84579302257402522</v>
       </c>
-      <c r="H30" s="28">
-        <f>F10/(F10+G10+H10)</f>
+      <c r="H30" s="25">
+        <f t="shared" si="3"/>
         <v>0.73297764227642281</v>
       </c>
-      <c r="I30" s="26">
-        <f>I10/(I10+J10)</f>
+      <c r="I30" s="23">
+        <f t="shared" si="4"/>
         <v>0.87917888563049851</v>
       </c>
-      <c r="J30" s="27">
-        <f>I10/(I10+K10)</f>
+      <c r="J30" s="24">
+        <f t="shared" si="5"/>
         <v>0.87892113749633538</v>
       </c>
-      <c r="K30" s="28">
-        <f>I10/(I10+J10+K10)</f>
+      <c r="K30" s="25">
+        <f t="shared" si="6"/>
         <v>0.78420088935391052</v>
       </c>
-      <c r="L30" s="37">
-        <f t="shared" si="1"/>
+      <c r="L30" s="34">
+        <f t="shared" si="7"/>
         <v>5.122324707748771E-2</v>
       </c>
-      <c r="M30" s="38">
+      <c r="M30" s="35">
         <v>3.6647727272727297E-2</v>
       </c>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
         <v>7</v>
       </c>
@@ -2858,39 +5199,39 @@
       <c r="E31" s="4">
         <v>3526</v>
       </c>
-      <c r="F31" s="26">
-        <f>F11/(F11+G11)</f>
+      <c r="F31" s="23">
+        <f t="shared" si="1"/>
         <v>0.7020818377602297</v>
       </c>
-      <c r="G31" s="27">
-        <f>F11/(F11+H11)</f>
+      <c r="G31" s="24">
+        <f t="shared" si="2"/>
         <v>0.55473624503686902</v>
       </c>
-      <c r="H31" s="28">
-        <f>F11/(F11+G11+H11)</f>
+      <c r="H31" s="25">
+        <f t="shared" si="3"/>
         <v>0.44903581267217629</v>
       </c>
-      <c r="I31" s="26">
-        <f>I11/(I11+J11)</f>
+      <c r="I31" s="23">
+        <f t="shared" si="4"/>
         <v>0.82555635319454412</v>
       </c>
-      <c r="J31" s="27">
-        <f>I11/(I11+K11)</f>
+      <c r="J31" s="24">
+        <f t="shared" si="5"/>
         <v>0.6522972206466251</v>
       </c>
-      <c r="K31" s="28">
-        <f>I11/(I11+J11+K11)</f>
+      <c r="K31" s="25">
+        <f t="shared" si="6"/>
         <v>0.57328015952143574</v>
       </c>
-      <c r="L31" s="37">
-        <f t="shared" si="1"/>
+      <c r="L31" s="34">
+        <f t="shared" si="7"/>
         <v>0.12424434684925945</v>
       </c>
-      <c r="M31" s="38">
+      <c r="M31" s="35">
         <v>3.3522727272727301E-2</v>
       </c>
     </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
         <v>8</v>
       </c>
@@ -2900,39 +5241,39 @@
       <c r="E32" s="4">
         <v>3383</v>
       </c>
-      <c r="F32" s="26">
-        <f>F12/(F12+G12)</f>
+      <c r="F32" s="23">
+        <f t="shared" si="1"/>
         <v>0.97892549718017219</v>
       </c>
-      <c r="G32" s="27">
-        <f>F12/(F12+H12)</f>
+      <c r="G32" s="24">
+        <f t="shared" si="2"/>
         <v>0.97487437185929648</v>
       </c>
-      <c r="H32" s="28">
-        <f>F12/(F12+G12+H12)</f>
+      <c r="H32" s="25">
+        <f t="shared" si="3"/>
         <v>0.95483497394325423</v>
       </c>
-      <c r="I32" s="26">
-        <f>I12/(I12+J12)</f>
+      <c r="I32" s="23">
+        <f t="shared" si="4"/>
         <v>0.99050163253190859</v>
       </c>
-      <c r="J32" s="27">
-        <f>I12/(I12+K12)</f>
+      <c r="J32" s="24">
+        <f t="shared" si="5"/>
         <v>0.98640260124150159</v>
       </c>
-      <c r="K32" s="28">
-        <f>I12/(I12+J12+K12)</f>
+      <c r="K32" s="25">
+        <f t="shared" si="6"/>
         <v>0.97715959004392383</v>
       </c>
-      <c r="L32" s="37">
-        <f t="shared" si="1"/>
+      <c r="L32" s="34">
+        <f t="shared" si="7"/>
         <v>2.2324616100669603E-2</v>
       </c>
-      <c r="M32" s="38">
+      <c r="M32" s="35">
         <v>3.2102272727272702E-2</v>
       </c>
     </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
         <v>9</v>
       </c>
@@ -2942,39 +5283,39 @@
       <c r="E33" s="4">
         <v>3448</v>
       </c>
-      <c r="F33" s="26">
-        <f>F13/(F13+G13)</f>
+      <c r="F33" s="23">
+        <f t="shared" si="1"/>
         <v>0.91798015178050207</v>
       </c>
-      <c r="G33" s="27">
-        <f>F13/(F13+H13)</f>
+      <c r="G33" s="24">
+        <f t="shared" si="2"/>
         <v>0.91212296983758701</v>
       </c>
-      <c r="H33" s="28">
-        <f>F13/(F13+G13+H13)</f>
+      <c r="H33" s="25">
+        <f t="shared" si="3"/>
         <v>0.84338964869938327</v>
       </c>
-      <c r="I33" s="26">
-        <f>I13/(I13+J13)</f>
+      <c r="I33" s="23">
+        <f t="shared" si="4"/>
         <v>0.92936368943374192</v>
       </c>
-      <c r="J33" s="27">
-        <f>I13/(I13+K13)</f>
+      <c r="J33" s="24">
+        <f t="shared" si="5"/>
         <v>0.92343387470997684</v>
       </c>
-      <c r="K33" s="28">
-        <f>I13/(I13+J13+K13)</f>
+      <c r="K33" s="25">
+        <f t="shared" si="6"/>
         <v>0.86287262872628723</v>
       </c>
-      <c r="L33" s="37">
-        <f t="shared" si="1"/>
+      <c r="L33" s="34">
+        <f t="shared" si="7"/>
         <v>1.9482980026903962E-2</v>
       </c>
-      <c r="M33" s="38">
+      <c r="M33" s="35">
         <v>2.75568181818182E-2</v>
       </c>
     </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="3" t="s">
         <v>10</v>
       </c>
@@ -2984,39 +5325,39 @@
       <c r="E34" s="4">
         <v>3472</v>
       </c>
-      <c r="F34" s="26">
-        <f>F14/(F14+G14)</f>
+      <c r="F34" s="23">
+        <f t="shared" si="1"/>
         <v>0.7054286561851083</v>
       </c>
-      <c r="G34" s="27">
-        <f>F14/(F14+H14)</f>
+      <c r="G34" s="24">
+        <f t="shared" si="2"/>
         <v>0.68490783410138245</v>
       </c>
-      <c r="H34" s="28">
-        <f>F14/(F14+G14+H14)</f>
+      <c r="H34" s="25">
+        <f t="shared" si="3"/>
         <v>0.53258678611422172</v>
       </c>
-      <c r="I34" s="26">
-        <f>I14/(I14+J14)</f>
+      <c r="I34" s="23">
+        <f t="shared" si="4"/>
         <v>0.83328389202017206</v>
       </c>
-      <c r="J34" s="27">
-        <f>I14/(I14+K14)</f>
+      <c r="J34" s="24">
+        <f t="shared" si="5"/>
         <v>0.80904377880184331</v>
       </c>
-      <c r="K34" s="28">
-        <f>I14/(I14+J14+K14)</f>
+      <c r="K34" s="25">
+        <f t="shared" si="6"/>
         <v>0.69633118492811108</v>
       </c>
-      <c r="L34" s="37">
-        <f t="shared" si="1"/>
+      <c r="L34" s="34">
+        <f t="shared" si="7"/>
         <v>0.16374439881388936</v>
       </c>
-      <c r="M34" s="38">
+      <c r="M34" s="35">
         <v>2.07386363636364E-2</v>
       </c>
     </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
@@ -3026,39 +5367,39 @@
       <c r="E35" s="4">
         <v>3414</v>
       </c>
-      <c r="F35" s="26">
-        <f>F15/(F15+G15)</f>
+      <c r="F35" s="23">
+        <f t="shared" si="1"/>
         <v>0.52840909090909094</v>
       </c>
-      <c r="G35" s="27">
-        <f>F15/(F15+H15)</f>
+      <c r="G35" s="24">
+        <f t="shared" si="2"/>
         <v>0.38137082601054484</v>
       </c>
-      <c r="H35" s="28">
-        <f>F15/(F15+G15+H15)</f>
+      <c r="H35" s="25">
+        <f t="shared" si="3"/>
         <v>0.28452797202797203</v>
       </c>
-      <c r="I35" s="26">
-        <f>I15/(I15+J15)</f>
+      <c r="I35" s="23">
+        <f t="shared" si="4"/>
         <v>0.67451298701298701</v>
       </c>
-      <c r="J35" s="27">
-        <f>I15/(I15+K15)</f>
+      <c r="J35" s="24">
+        <f t="shared" si="5"/>
         <v>0.4868189806678383</v>
       </c>
-      <c r="K35" s="28">
-        <f>I15/(I15+J15+K15)</f>
+      <c r="K35" s="25">
+        <f t="shared" si="6"/>
         <v>0.3942125237191651</v>
       </c>
-      <c r="L35" s="37">
-        <f t="shared" si="1"/>
+      <c r="L35" s="34">
+        <f t="shared" si="7"/>
         <v>0.10968455169119307</v>
       </c>
-      <c r="M35" s="38">
+      <c r="M35" s="35">
         <v>1.19318181818182E-2</v>
       </c>
     </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
         <v>12</v>
       </c>
@@ -3068,39 +5409,39 @@
       <c r="E36" s="4">
         <v>3364</v>
       </c>
-      <c r="F36" s="26">
-        <f>F16/(F16+G16)</f>
+      <c r="F36" s="23">
+        <f t="shared" si="1"/>
         <v>0.94660338178582026</v>
       </c>
-      <c r="G36" s="27">
-        <f>F16/(F16+H16)</f>
+      <c r="G36" s="24">
+        <f t="shared" si="2"/>
         <v>0.94857312722948872</v>
       </c>
-      <c r="H36" s="28">
-        <f>F16/(F16+G16+H16)</f>
+      <c r="H36" s="25">
+        <f t="shared" si="3"/>
         <v>0.90039503386004516</v>
       </c>
-      <c r="I36" s="26">
-        <f>I16/(I16+J16)</f>
+      <c r="I36" s="23">
+        <f t="shared" si="4"/>
         <v>0.97745476119845742</v>
       </c>
-      <c r="J36" s="27">
-        <f>I16/(I16+K16)</f>
+      <c r="J36" s="24">
+        <f t="shared" si="5"/>
         <v>0.97948870392390008</v>
       </c>
-      <c r="K36" s="28">
-        <f>I16/(I16+J16+K16)</f>
+      <c r="K36" s="25">
+        <f t="shared" si="6"/>
         <v>0.95784883720930236</v>
       </c>
-      <c r="L36" s="37">
-        <f t="shared" si="1"/>
+      <c r="L36" s="34">
+        <f t="shared" si="7"/>
         <v>5.7453803349257204E-2</v>
       </c>
-      <c r="M36" s="38">
+      <c r="M36" s="35">
         <v>3.9488636363636399E-2</v>
       </c>
     </row>
-    <row r="37" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C37" s="3" t="s">
         <v>13</v>
       </c>
@@ -3110,39 +5451,39 @@
       <c r="E37" s="4">
         <v>3462</v>
       </c>
-      <c r="F37" s="26">
-        <f>F17/(F17+G17)</f>
+      <c r="F37" s="23">
+        <f t="shared" si="1"/>
         <v>0.78005188815220527</v>
       </c>
-      <c r="G37" s="27">
-        <f>F17/(F17+H17)</f>
+      <c r="G37" s="24">
+        <f t="shared" si="2"/>
         <v>0.78162911611785091</v>
       </c>
-      <c r="H37" s="28">
-        <f>F17/(F17+G17+H17)</f>
+      <c r="H37" s="25">
+        <f t="shared" si="3"/>
         <v>0.64047337278106509</v>
       </c>
-      <c r="I37" s="26">
-        <f>I17/(I17+J17)</f>
+      <c r="I37" s="23">
+        <f t="shared" si="4"/>
         <v>0.82069760737964836</v>
       </c>
-      <c r="J37" s="27">
-        <f>I17/(I17+K17)</f>
+      <c r="J37" s="24">
+        <f t="shared" si="5"/>
         <v>0.82235701906412473</v>
       </c>
-      <c r="K37" s="28">
-        <f>I17/(I17+J17+K17)</f>
+      <c r="K37" s="25">
+        <f t="shared" si="6"/>
         <v>0.69711067580803132</v>
       </c>
-      <c r="L37" s="37">
-        <f t="shared" si="1"/>
+      <c r="L37" s="34">
+        <f t="shared" si="7"/>
         <v>5.6637303026966235E-2</v>
       </c>
-      <c r="M37" s="38">
+      <c r="M37" s="35">
         <v>3.2102272727272702E-2</v>
       </c>
     </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C38" s="3" t="s">
         <v>14</v>
       </c>
@@ -3152,39 +5493,39 @@
       <c r="E38" s="4">
         <v>3440</v>
       </c>
-      <c r="F38" s="26">
-        <f>F18/(F18+G18)</f>
+      <c r="F38" s="23">
+        <f t="shared" si="1"/>
         <v>0.70855457227138641</v>
       </c>
-      <c r="G38" s="27">
-        <f>F18/(F18+H18)</f>
+      <c r="G38" s="24">
+        <f t="shared" si="2"/>
         <v>0.69825581395348835</v>
       </c>
-      <c r="H38" s="28">
-        <f>F18/(F18+G18+H18)</f>
+      <c r="H38" s="25">
+        <f t="shared" si="3"/>
         <v>0.54245709123757901</v>
       </c>
-      <c r="I38" s="26">
-        <f>I18/(I18+J18)</f>
+      <c r="I38" s="23">
+        <f t="shared" si="4"/>
         <v>0.73244837758112091</v>
       </c>
-      <c r="J38" s="27">
-        <f>I18/(I18+K18)</f>
+      <c r="J38" s="24">
+        <f t="shared" si="5"/>
         <v>0.72180232558139534</v>
       </c>
-      <c r="K38" s="28">
-        <f>I18/(I18+J18+K18)</f>
+      <c r="K38" s="25">
+        <f t="shared" si="6"/>
         <v>0.5711985277202668</v>
       </c>
-      <c r="L38" s="37">
-        <f t="shared" si="1"/>
+      <c r="L38" s="34">
+        <f t="shared" si="7"/>
         <v>2.8741436482687788E-2</v>
       </c>
-      <c r="M38" s="38">
+      <c r="M38" s="35">
         <v>2.61363636363636E-2</v>
       </c>
     </row>
-    <row r="39" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C39" s="3" t="s">
         <v>15</v>
       </c>
@@ -3194,73 +5535,73 @@
       <c r="E39" s="4">
         <v>3493</v>
       </c>
-      <c r="F39" s="29">
-        <f>F19/(F19+G19)</f>
+      <c r="F39" s="26">
+        <f t="shared" si="1"/>
         <v>0.65016747301823596</v>
       </c>
-      <c r="G39" s="30">
-        <f>F19/(F19+H19)</f>
+      <c r="G39" s="27">
+        <f t="shared" si="2"/>
         <v>0.50014314342971655</v>
       </c>
-      <c r="H39" s="31">
-        <f>F19/(F19+G19+H19)</f>
+      <c r="H39" s="28">
+        <f t="shared" si="3"/>
         <v>0.39408978118655535</v>
       </c>
-      <c r="I39" s="29">
-        <f>I19/(I19+J19)</f>
+      <c r="I39" s="26">
+        <f t="shared" si="4"/>
         <v>0.72050614067733532</v>
       </c>
-      <c r="J39" s="30">
-        <f>I19/(I19+K19)</f>
+      <c r="J39" s="27">
+        <f t="shared" si="5"/>
         <v>0.55425135986258234</v>
       </c>
-      <c r="K39" s="31">
-        <f>I19/(I19+J19+K19)</f>
+      <c r="K39" s="28">
+        <f t="shared" si="6"/>
         <v>0.45617342130065974</v>
       </c>
-      <c r="L39" s="37">
-        <f t="shared" si="1"/>
+      <c r="L39" s="34">
+        <f t="shared" si="7"/>
         <v>6.2083640114104388E-2</v>
       </c>
-      <c r="M39" s="38">
+      <c r="M39" s="35">
         <v>2.07386363636364E-2</v>
       </c>
     </row>
-    <row r="40" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C40" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="32">
+      <c r="F40" s="29">
         <f>AVERAGE(F24:F39)</f>
         <v>0.85309609700624933</v>
       </c>
-      <c r="G40" s="33">
+      <c r="G40" s="30">
         <f>AVERAGE(G24:G39)</f>
         <v>0.781871868967418</v>
       </c>
-      <c r="H40" s="33">
-        <f t="shared" ref="H40:K40" si="2">AVERAGE(H24:H39)</f>
+      <c r="H40" s="30">
+        <f t="shared" ref="H40:K40" si="8">AVERAGE(H24:H39)</f>
         <v>0.71350322084923956</v>
       </c>
-      <c r="I40" s="33">
-        <f t="shared" si="2"/>
+      <c r="I40" s="30">
+        <f t="shared" si="8"/>
         <v>0.89365126911520687</v>
       </c>
-      <c r="J40" s="33">
-        <f t="shared" si="2"/>
+      <c r="J40" s="30">
+        <f t="shared" si="8"/>
         <v>0.81664331039494042</v>
       </c>
-      <c r="K40" s="34">
-        <f t="shared" si="2"/>
+      <c r="K40" s="31">
+        <f t="shared" si="8"/>
         <v>0.75967105956607983</v>
       </c>
-      <c r="L40" s="36">
+      <c r="L40" s="33">
         <f>MEDIAN(L24:L39)</f>
         <v>2.5533026291678695E-2</v>
       </c>
-      <c r="M40" s="36">
+      <c r="M40" s="33">
         <f>MEDIAN(M24:M39)</f>
         <v>2.68465909090909E-2</v>
       </c>

</xml_diff>